<commit_message>
UPDATE: Refactor and change optional for use_serde cfg
</commit_message>
<xml_diff>
--- a/tests/files/test_excel.xlsx
+++ b/tests/files/test_excel.xlsx
@@ -419,2002 +419,2002 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B2">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E2">
         <v>420</v>
       </c>
       <c r="F2" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B3">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E3">
         <v>420</v>
       </c>
       <c r="F3" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B4">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E4">
         <v>420</v>
       </c>
       <c r="F4" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B5">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E5">
         <v>420</v>
       </c>
       <c r="F5" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B6">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E6">
         <v>420</v>
       </c>
       <c r="F6" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B7">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E7">
         <v>420</v>
       </c>
       <c r="F7" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B8">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E8">
         <v>420</v>
       </c>
       <c r="F8" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B9">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E9">
         <v>420</v>
       </c>
       <c r="F9" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B10">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E10">
         <v>420</v>
       </c>
       <c r="F10" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B11">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E11">
         <v>420</v>
       </c>
       <c r="F11" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B12">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E12">
         <v>420</v>
       </c>
       <c r="F12" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B13">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E13">
         <v>420</v>
       </c>
       <c r="F13" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B14">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E14">
         <v>420</v>
       </c>
       <c r="F14" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B15">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E15">
         <v>420</v>
       </c>
       <c r="F15" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B16">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E16">
         <v>420</v>
       </c>
       <c r="F16" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B17">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E17">
         <v>420</v>
       </c>
       <c r="F17" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B18">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E18">
         <v>420</v>
       </c>
       <c r="F18" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B19">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E19">
         <v>420</v>
       </c>
       <c r="F19" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B20">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E20">
         <v>420</v>
       </c>
       <c r="F20" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B21">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E21">
         <v>420</v>
       </c>
       <c r="F21" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B22">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E22">
         <v>420</v>
       </c>
       <c r="F22" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B23">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E23">
         <v>420</v>
       </c>
       <c r="F23" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B24">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E24">
         <v>420</v>
       </c>
       <c r="F24" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B25">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E25">
         <v>420</v>
       </c>
       <c r="F25" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B26">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E26">
         <v>420</v>
       </c>
       <c r="F26" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B27">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E27">
         <v>420</v>
       </c>
       <c r="F27" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B28">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E28">
         <v>420</v>
       </c>
       <c r="F28" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B29">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E29">
         <v>420</v>
       </c>
       <c r="F29" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B30">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E30">
         <v>420</v>
       </c>
       <c r="F30" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B31">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E31">
         <v>420</v>
       </c>
       <c r="F31" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B32">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E32">
         <v>420</v>
       </c>
       <c r="F32" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B33">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E33">
         <v>420</v>
       </c>
       <c r="F33" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B34">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E34">
         <v>420</v>
       </c>
       <c r="F34" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B35">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E35">
         <v>420</v>
       </c>
       <c r="F35" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B36">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E36">
         <v>420</v>
       </c>
       <c r="F36" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B37">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E37">
         <v>420</v>
       </c>
       <c r="F37" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B38">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E38">
         <v>420</v>
       </c>
       <c r="F38" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B39">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E39">
         <v>420</v>
       </c>
       <c r="F39" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B40">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E40">
         <v>420</v>
       </c>
       <c r="F40" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B41">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E41">
         <v>420</v>
       </c>
       <c r="F41" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B42">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E42">
         <v>420</v>
       </c>
       <c r="F42" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B43">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E43">
         <v>420</v>
       </c>
       <c r="F43" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B44">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E44">
         <v>420</v>
       </c>
       <c r="F44" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B45">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E45">
         <v>420</v>
       </c>
       <c r="F45" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B46">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E46">
         <v>420</v>
       </c>
       <c r="F46" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B47">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E47">
         <v>420</v>
       </c>
       <c r="F47" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B48">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E48">
         <v>420</v>
       </c>
       <c r="F48" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B49">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E49">
         <v>420</v>
       </c>
       <c r="F49" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B50">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E50">
         <v>420</v>
       </c>
       <c r="F50" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B51">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E51">
         <v>420</v>
       </c>
       <c r="F51" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B52">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E52">
         <v>420</v>
       </c>
       <c r="F52" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B53">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E53">
         <v>420</v>
       </c>
       <c r="F53" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B54">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E54">
         <v>420</v>
       </c>
       <c r="F54" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B55">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E55">
         <v>420</v>
       </c>
       <c r="F55" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B56">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E56">
         <v>420</v>
       </c>
       <c r="F56" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B57">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E57">
         <v>420</v>
       </c>
       <c r="F57" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B58">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E58">
         <v>420</v>
       </c>
       <c r="F58" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B59">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E59">
         <v>420</v>
       </c>
       <c r="F59" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B60">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E60">
         <v>420</v>
       </c>
       <c r="F60" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B61">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E61">
         <v>420</v>
       </c>
       <c r="F61" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B62">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E62">
         <v>420</v>
       </c>
       <c r="F62" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B63">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E63">
         <v>420</v>
       </c>
       <c r="F63" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B64">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E64">
         <v>420</v>
       </c>
       <c r="F64" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B65">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E65">
         <v>420</v>
       </c>
       <c r="F65" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B66">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E66">
         <v>420</v>
       </c>
       <c r="F66" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B67">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E67">
         <v>420</v>
       </c>
       <c r="F67" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B68">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E68">
         <v>420</v>
       </c>
       <c r="F68" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B69">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E69">
         <v>420</v>
       </c>
       <c r="F69" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B70">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E70">
         <v>420</v>
       </c>
       <c r="F70" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B71">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E71">
         <v>420</v>
       </c>
       <c r="F71" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B72">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E72">
         <v>420</v>
       </c>
       <c r="F72" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B73">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E73">
         <v>420</v>
       </c>
       <c r="F73" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B74">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E74">
         <v>420</v>
       </c>
       <c r="F74" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B75">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E75">
         <v>420</v>
       </c>
       <c r="F75" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B76">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E76">
         <v>420</v>
       </c>
       <c r="F76" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B77">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E77">
         <v>420</v>
       </c>
       <c r="F77" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B78">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E78">
         <v>420</v>
       </c>
       <c r="F78" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B79">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E79">
         <v>420</v>
       </c>
       <c r="F79" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B80">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E80">
         <v>420</v>
       </c>
       <c r="F80" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B81">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E81">
         <v>420</v>
       </c>
       <c r="F81" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B82">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E82">
         <v>420</v>
       </c>
       <c r="F82" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B83">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E83">
         <v>420</v>
       </c>
       <c r="F83" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B84">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E84">
         <v>420</v>
       </c>
       <c r="F84" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B85">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E85">
         <v>420</v>
       </c>
       <c r="F85" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B86">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E86">
         <v>420</v>
       </c>
       <c r="F86" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B87">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E87">
         <v>420</v>
       </c>
       <c r="F87" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B88">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E88">
         <v>420</v>
       </c>
       <c r="F88" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B89">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E89">
         <v>420</v>
       </c>
       <c r="F89" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B90">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E90">
         <v>420</v>
       </c>
       <c r="F90" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B91">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E91">
         <v>420</v>
       </c>
       <c r="F91" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B92">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E92">
         <v>420</v>
       </c>
       <c r="F92" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B93">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E93">
         <v>420</v>
       </c>
       <c r="F93" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B94">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E94">
         <v>420</v>
       </c>
       <c r="F94" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B95">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E95">
         <v>420</v>
       </c>
       <c r="F95" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B96">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E96">
         <v>420</v>
       </c>
       <c r="F96" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B97">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E97">
         <v>420</v>
       </c>
       <c r="F97" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B98">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E98">
         <v>420</v>
       </c>
       <c r="F98" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B99">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E99">
         <v>420</v>
       </c>
       <c r="F99" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B100">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E100">
         <v>420</v>
       </c>
       <c r="F100" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>105.55742871467407</v>
+        <v>88.45342611741277</v>
       </c>
       <c r="B101">
-        <v>20699.9586000828</v>
+        <v>41399.9172001656</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>569.0215447350218</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>2467.006475771309</v>
       </c>
       <c r="E101">
         <v>420</v>
       </c>
       <c r="F101" s="2">
-        <v>45025.03367445602</v>
+        <v>45055.898259560185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>